<commit_message>
- Reallocation of components to have a view after the change to I2C components - Update BOM with costs
</commit_message>
<xml_diff>
--- a/Connect Medical Boards/EFM1/Project Outputs for 105358-3BA001-01_EFM1/105358-3BA001-03_EFM1_BOM.xlsx
+++ b/Connect Medical Boards/EFM1/Project Outputs for 105358-3BA001-01_EFM1/105358-3BA001-03_EFM1_BOM.xlsx
@@ -3,13 +3,18 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\Connect Medical Boards\EFM1\Project Outputs for 105358-3BA001-01_EFM1\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="11595"/>
   </bookViews>
   <sheets>
     <sheet name="105358-3BA001-03_EFM1_BOM" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="152511" refMode="R1C1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="172">
   <si>
     <t>Designator</t>
   </si>
@@ -354,16 +359,16 @@
     <t>R6</t>
   </si>
   <si>
-    <t>RES SMD 8.2kOHM 5% 1/16W 0402</t>
-  </si>
-  <si>
-    <t>8.2K</t>
-  </si>
-  <si>
-    <t>RC0402JR-078K2L</t>
-  </si>
-  <si>
-    <t>311-8.2KJRCT-ND</t>
+    <t>RES SMD 5.6kOHM 5% 1/16W 0402</t>
+  </si>
+  <si>
+    <t>5.6K</t>
+  </si>
+  <si>
+    <t>RC0402JR-075K6L</t>
+  </si>
+  <si>
+    <t>311-5.6KJRCT-ND</t>
   </si>
   <si>
     <t>R7</t>
@@ -514,6 +519,27 @@
   </si>
   <si>
     <t>12-XFQFN</t>
+  </si>
+  <si>
+    <t>Total Cost</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>(Cost @10k by William)</t>
+  </si>
+  <si>
+    <t>Cost as 20170816 (unit)</t>
+  </si>
+  <si>
+    <t>Cost as 20170816 (K-uni`t)</t>
+  </si>
+  <si>
+    <t>CKN10777CT-ND</t>
   </si>
 </sst>
 </file>
@@ -549,7 +575,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -572,17 +598,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -863,9 +903,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I30"/>
+  <dimension ref="A1:M31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="M23" sqref="M23"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -877,9 +919,12 @@
     <col min="6" max="6" width="31.140625" customWidth="1"/>
     <col min="7" max="7" width="31" customWidth="1"/>
     <col min="8" max="9" width="14.42578125" customWidth="1"/>
+    <col min="10" max="10" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -907,8 +952,17 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
@@ -936,8 +990,18 @@
       <c r="I2" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J2" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="K2" s="3">
+        <v>8.7600000000000004E-3</v>
+      </c>
+      <c r="L2" s="2">
+        <f>K2*H2</f>
+        <v>5.2560000000000003E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>17</v>
       </c>
@@ -965,8 +1029,18 @@
       <c r="I3" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J3" s="3">
+        <v>0.46</v>
+      </c>
+      <c r="K3" s="3">
+        <v>0.12018</v>
+      </c>
+      <c r="L3" s="2">
+        <f t="shared" ref="L3:L29" si="0">K3*H3</f>
+        <v>0.48071999999999998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>23</v>
       </c>
@@ -994,8 +1068,18 @@
       <c r="I4" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J4" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="K4" s="3">
+        <v>0.13219</v>
+      </c>
+      <c r="L4" s="2">
+        <f t="shared" si="0"/>
+        <v>0.26438</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>30</v>
       </c>
@@ -1023,8 +1107,18 @@
       <c r="I5" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J5" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="K5" s="3">
+        <v>6.62E-3</v>
+      </c>
+      <c r="L5" s="2">
+        <f t="shared" si="0"/>
+        <v>6.62E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>35</v>
       </c>
@@ -1052,8 +1146,18 @@
       <c r="I6" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J6" s="3">
+        <v>0.26</v>
+      </c>
+      <c r="K6" s="3">
+        <v>5.5280000000000003E-2</v>
+      </c>
+      <c r="L6" s="2">
+        <f t="shared" si="0"/>
+        <v>0.11056000000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>41</v>
       </c>
@@ -1081,8 +1185,18 @@
       <c r="I7" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J7" s="3">
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="K7" s="3">
+        <v>0.71874000000000005</v>
+      </c>
+      <c r="L7" s="2">
+        <f t="shared" si="0"/>
+        <v>0.71874000000000005</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>46</v>
       </c>
@@ -1110,8 +1224,18 @@
       <c r="I8" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J8" s="3">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="K8" s="3">
+        <v>0.29712</v>
+      </c>
+      <c r="L8" s="2">
+        <f t="shared" si="0"/>
+        <v>0.29712</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>51</v>
       </c>
@@ -1139,8 +1263,18 @@
       <c r="I9" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J9" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="K9" s="3">
+        <v>7.4459999999999998E-2</v>
+      </c>
+      <c r="L9" s="2">
+        <f t="shared" si="0"/>
+        <v>7.4459999999999998E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>54</v>
       </c>
@@ -1168,8 +1302,18 @@
       <c r="I10" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J10" s="3">
+        <v>0.49</v>
+      </c>
+      <c r="K10" s="3">
+        <v>0.1144</v>
+      </c>
+      <c r="L10" s="2">
+        <f t="shared" si="0"/>
+        <v>0.1144</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>59</v>
       </c>
@@ -1197,8 +1341,18 @@
       <c r="I11" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J11" s="3">
+        <v>0.33</v>
+      </c>
+      <c r="K11" s="3">
+        <v>0.154</v>
+      </c>
+      <c r="L11" s="2">
+        <f t="shared" si="0"/>
+        <v>0.154</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>64</v>
       </c>
@@ -1226,8 +1380,18 @@
       <c r="I12" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J12" s="3">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="K12" s="3">
+        <v>6.0380000000000003E-2</v>
+      </c>
+      <c r="L12" s="2">
+        <f t="shared" si="0"/>
+        <v>6.0380000000000003E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>70</v>
       </c>
@@ -1255,8 +1419,18 @@
       <c r="I13" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J13" s="3">
+        <v>0.21</v>
+      </c>
+      <c r="K13" s="3">
+        <v>8.6459999999999995E-2</v>
+      </c>
+      <c r="L13" s="2">
+        <f t="shared" si="0"/>
+        <v>8.6459999999999995E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>75</v>
       </c>
@@ -1284,8 +1458,18 @@
       <c r="I14" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J14" s="3">
+        <v>0.12</v>
+      </c>
+      <c r="K14" s="3">
+        <v>3.0620000000000001E-2</v>
+      </c>
+      <c r="L14" s="2">
+        <f t="shared" si="0"/>
+        <v>3.0620000000000001E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>80</v>
       </c>
@@ -1313,8 +1497,21 @@
       <c r="I15" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J15" s="3">
+        <v>14.72</v>
+      </c>
+      <c r="K15" s="3">
+        <v>4</v>
+      </c>
+      <c r="L15" s="2">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="M15" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>85</v>
       </c>
@@ -1342,8 +1539,18 @@
       <c r="I16" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J16" s="3">
+        <v>0.49</v>
+      </c>
+      <c r="K16" s="3">
+        <v>0.1144</v>
+      </c>
+      <c r="L16" s="2">
+        <f t="shared" si="0"/>
+        <v>0.1144</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>89</v>
       </c>
@@ -1371,8 +1578,18 @@
       <c r="I17" s="2" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J17" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="K17" s="3">
+        <v>2.47E-3</v>
+      </c>
+      <c r="L17" s="2">
+        <f t="shared" si="0"/>
+        <v>2.47E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>95</v>
       </c>
@@ -1400,8 +1617,18 @@
       <c r="I18" s="2" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J18" s="3">
+        <v>0.11</v>
+      </c>
+      <c r="K18" s="3">
+        <v>2.66E-3</v>
+      </c>
+      <c r="L18" s="2">
+        <f t="shared" si="0"/>
+        <v>2.66E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>100</v>
       </c>
@@ -1429,8 +1656,18 @@
       <c r="I19" s="2" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J19" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="K19" s="3">
+        <v>4.4799999999999996E-3</v>
+      </c>
+      <c r="L19" s="2">
+        <f t="shared" si="0"/>
+        <v>8.9599999999999992E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>105</v>
       </c>
@@ -1458,8 +1695,18 @@
       <c r="I20" s="2" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J20" s="3">
+        <v>0.11</v>
+      </c>
+      <c r="K20" s="3">
+        <v>2.66E-3</v>
+      </c>
+      <c r="L20" s="2">
+        <f t="shared" si="0"/>
+        <v>1.064E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>110</v>
       </c>
@@ -1487,8 +1734,18 @@
       <c r="I21" s="2" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J21" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="K21" s="3">
+        <v>2.2399999999999998E-3</v>
+      </c>
+      <c r="L21" s="2">
+        <f t="shared" si="0"/>
+        <v>2.2399999999999998E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>115</v>
       </c>
@@ -1516,8 +1773,18 @@
       <c r="I22" s="2" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J22" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="K22" s="3">
+        <v>2.47E-3</v>
+      </c>
+      <c r="L22" s="2">
+        <f t="shared" si="0"/>
+        <v>2.47E-3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>120</v>
       </c>
@@ -1545,8 +1812,18 @@
       <c r="I23" s="2" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J23" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="K23" s="3">
+        <v>2.47E-3</v>
+      </c>
+      <c r="L23" s="2">
+        <f t="shared" si="0"/>
+        <v>2.47E-3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>125</v>
       </c>
@@ -1574,8 +1851,18 @@
       <c r="I24" s="2" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J24" s="3">
+        <v>0.11</v>
+      </c>
+      <c r="K24" s="3">
+        <v>2.66E-3</v>
+      </c>
+      <c r="L24" s="2">
+        <f t="shared" si="0"/>
+        <v>2.66E-3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>130</v>
       </c>
@@ -1592,7 +1879,7 @@
         <v>134</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>16</v>
+        <v>171</v>
       </c>
       <c r="G25" s="2" t="s">
         <v>16</v>
@@ -1603,8 +1890,18 @@
       <c r="I25" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J25" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="K25" s="3">
+        <v>0.14438000000000001</v>
+      </c>
+      <c r="L25" s="2">
+        <f t="shared" si="0"/>
+        <v>0.28876000000000002</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>135</v>
       </c>
@@ -1632,8 +1929,18 @@
       <c r="I26" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J26" s="3">
+        <v>1.28</v>
+      </c>
+      <c r="K26" s="3">
+        <v>0.58401000000000003</v>
+      </c>
+      <c r="L26" s="2">
+        <f t="shared" si="0"/>
+        <v>0.58401000000000003</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>141</v>
       </c>
@@ -1661,8 +1968,18 @@
       <c r="I27" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J27" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="K27" s="3">
+        <v>1.4490000000000001</v>
+      </c>
+      <c r="L27" s="2">
+        <f t="shared" si="0"/>
+        <v>1.4490000000000001</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>146</v>
       </c>
@@ -1690,8 +2007,18 @@
       <c r="I28" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J28" s="3">
+        <v>2.86</v>
+      </c>
+      <c r="K28" s="3">
+        <v>1.4038900000000001</v>
+      </c>
+      <c r="L28" s="2">
+        <f t="shared" si="0"/>
+        <v>1.4038900000000001</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>153</v>
       </c>
@@ -1719,8 +2046,18 @@
       <c r="I29" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J29" s="3">
+        <v>0.37</v>
+      </c>
+      <c r="K29" s="3">
+        <v>0.28148000000000001</v>
+      </c>
+      <c r="L29" s="2">
+        <f t="shared" ref="L29" si="1">K29*H29</f>
+        <v>0.28148000000000001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>159</v>
       </c>
@@ -1747,6 +2084,25 @@
       </c>
       <c r="I30" s="2" t="s">
         <v>16</v>
+      </c>
+      <c r="J30" s="3">
+        <v>0.85</v>
+      </c>
+      <c r="K30" s="3">
+        <v>0.38624999999999998</v>
+      </c>
+      <c r="L30" s="3">
+        <f>K30*H29</f>
+        <v>0.38624999999999998</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K31" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="L31" s="3">
+        <f>SUM(L2:L30)</f>
+        <v>10.99338</v>
       </c>
     </row>
   </sheetData>

</xml_diff>